<commit_message>
working on excel sumif
</commit_message>
<xml_diff>
--- a/rx_PSC_RentalActivity.xlsx
+++ b/rx_PSC_RentalActivity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BerilP\repos\PSC-RentalActivity-YSR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B88F22D2-C406-4D92-B8F6-B4C92B6B3164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B5BFAA-5746-408B-8A65-D7A2210D8ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="380" windowWidth="19180" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PS" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,25 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">PS!$1:$4</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Rental Activity</t>
   </si>
@@ -67,12 +80,6 @@
     <t>Occ. %</t>
   </si>
   <si>
-    <t>Total for - 964SADDR1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grand total - </t>
-  </si>
-  <si>
     <t>&amp;=display.UnitType</t>
   </si>
   <si>
@@ -122,6 +129,48 @@
   </si>
   <si>
     <t>&amp;=header.ReportDateRange</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUM(D5:D{-1})</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUM(E5:E{-1})</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUM(F5:F{-1})</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUM(G5:G{-1})</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUM(H5:H{-1})</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUM(I5:I{-1})</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUM(J5:J{-1})</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUM(K5:K{-1})</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUM(L5:L{-1})</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUM(M5:M{-1})/100</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, C5:C{-1})</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=IF(A5=A{-1}, "dup","first")</t>
   </si>
 </sst>
 </file>
@@ -219,13 +268,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -552,213 +603,229 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7265625" customWidth="1"/>
-    <col min="3" max="3" width="9.54296875" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" customWidth="1"/>
-    <col min="5" max="5" width="8.453125" customWidth="1"/>
-    <col min="6" max="6" width="9.7265625" customWidth="1"/>
-    <col min="7" max="7" width="7.54296875" customWidth="1"/>
-    <col min="8" max="8" width="7.81640625" customWidth="1"/>
-    <col min="9" max="11" width="12.7265625" customWidth="1"/>
-    <col min="12" max="12" width="9.26953125" customWidth="1"/>
-    <col min="13" max="13" width="6.26953125" customWidth="1"/>
-    <col min="14" max="14" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="14.26953125" customWidth="1"/>
+    <col min="3" max="3" width="7.7265625" customWidth="1"/>
+    <col min="4" max="4" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" customWidth="1"/>
+    <col min="6" max="6" width="8.453125" customWidth="1"/>
+    <col min="7" max="7" width="9.7265625" customWidth="1"/>
+    <col min="8" max="8" width="7.54296875" customWidth="1"/>
+    <col min="9" max="9" width="7.81640625" customWidth="1"/>
+    <col min="10" max="12" width="12.7265625" customWidth="1"/>
+    <col min="13" max="13" width="9.26953125" customWidth="1"/>
+    <col min="14" max="14" width="6.26953125" customWidth="1"/>
+    <col min="15" max="15" width="21.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
     </row>
-    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
+    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
     </row>
-    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
+    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
     </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="5" t="s">
-        <v>30</v>
+      <c r="O4" s="4" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="L5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="M5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="N5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="M5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
+    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="O6" s="3"/>
     </row>
-    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="A2:N2"/>
-    <mergeCell ref="A3:N3"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A6:B6"/>
+  <mergeCells count="4">
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A3:O3"/>
+    <mergeCell ref="A6:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.7" bottom="0.7" header="0.5" footer="0.5"/>
   <pageSetup fitToHeight="990" orientation="portrait" useFirstPageNumber="1"/>
@@ -767,10 +834,10 @@
     <oddFooter>&amp;C&amp;B Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="30" max="16383" man="1"/>
+    <brk id="29" max="16383" man="1"/>
   </rowBreaks>
   <ignoredErrors>
-    <ignoredError sqref="A4:M4 A6:B7 A1" numberStoredAsText="1"/>
+    <ignoredError sqref="C4:N4 C6 A1 A4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Separate columns for vacant and unavailable
</commit_message>
<xml_diff>
--- a/rx_PSC_RentalActivity.xlsx
+++ b/rx_PSC_RentalActivity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BerilP\repos\PSC-RentalActivity-YSR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B5BFAA-5746-408B-8A65-D7A2210D8ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84738B3-7C0F-4D5A-B350-C6A4BA7F8DC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="380" windowWidth="19180" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2730" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PS" sheetId="1" r:id="rId1"/>
@@ -137,9 +137,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>&amp;=&amp;=SUM(D5:D{-1})</t>
-  </si>
-  <si>
     <t>&amp;=&amp;=SUM(E5:E{-1})</t>
   </si>
   <si>
@@ -164,13 +161,16 @@
     <t>&amp;=&amp;=SUM(L5:L{-1})</t>
   </si>
   <si>
-    <t>&amp;=&amp;=SUM(M5:M{-1})/100</t>
-  </si>
-  <si>
-    <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, C5:C{-1})</t>
-  </si>
-  <si>
-    <t>&amp;=&amp;=IF(A5=A{-1}, "dup","first")</t>
+    <t>&amp;=&amp;=IF(A5=A{-1}, 0,1)</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUMIF(B5:B{-1}, 1, D5:D{-1})</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUM(M5:M{-1})</t>
+  </si>
+  <si>
+    <t>&amp;=&amp;=SUM(N5:N{-1})/100</t>
   </si>
 </sst>
 </file>
@@ -606,14 +606,15 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="14.26953125" customWidth="1"/>
+    <col min="1" max="1" width="14.26953125" customWidth="1"/>
+    <col min="2" max="2" width="23.36328125" customWidth="1"/>
     <col min="3" max="3" width="7.7265625" customWidth="1"/>
-    <col min="4" max="4" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.6328125" customWidth="1"/>
     <col min="5" max="5" width="8.7265625" customWidth="1"/>
     <col min="6" max="6" width="8.453125" customWidth="1"/>
     <col min="7" max="7" width="9.7265625" customWidth="1"/>
@@ -732,7 +733,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>15</v>
@@ -781,7 +782,7 @@
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
       <c r="D6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>33</v>
@@ -808,10 +809,10 @@
         <v>40</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="O6" s="3"/>
     </row>

</xml_diff>